<commit_message>
manage cases: If A.Cell=blank or null Then A.Cell=blank or null
</commit_message>
<xml_diff>
--- a/2-Tests/Lexerow.Core.Tests/10-Files/Run/datLinesACellEqualBlankOk.xlsx
+++ b/2-Tests/Lexerow.Core.Tests/10-Files/Run/datLinesACellEqualBlankOk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylawr\OneDrive\ProjetsDev\10-Pierlam\Lexerow\Dev\Lexerow\2-Tests\Lexerow.Core.Tests\10-Files\Run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAF7A90-2B9D-43D6-A87C-DFD727360BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18803CF3-900D-4A21-9E05-83B40D464F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="1470" windowWidth="25155" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="2160" windowWidth="18720" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -376,7 +376,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>